<commit_message>
Added functionality PDF to Powerpoint completed
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484B023B-40D7-46AC-B1E0-38DDD7D11A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4ACB70-BD26-495F-8150-72C207F9B002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
   <si>
     <t>Feature</t>
   </si>
@@ -809,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -824,7 +824,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1143,7 +1142,7 @@
   <dimension ref="G4:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1238,7 +1237,7 @@
       <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1255,7 +1254,9 @@
       <c r="J9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="7:11" ht="28.8">
       <c r="G10" s="2" t="s">
@@ -1270,7 +1271,7 @@
       <c r="J10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="7"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="7:11" ht="27.6">
       <c r="G11" s="2" t="s">
@@ -1302,7 +1303,7 @@
       <c r="J12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="7"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="7:11">
       <c r="G13" s="2" t="s">
@@ -1317,7 +1318,7 @@
       <c r="J13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="7"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="7:11" ht="28.8">
       <c r="G14" s="2" t="s">
@@ -1332,7 +1333,7 @@
       <c r="J14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="7"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="7:11" ht="28.8">
       <c r="G15" s="2" t="s">
@@ -1347,7 +1348,7 @@
       <c r="J15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="7"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="7:11">
       <c r="G16" s="2" t="s">
@@ -1362,7 +1363,7 @@
       <c r="J16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="7"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="7:11" ht="28.8">
       <c r="G17" s="2" t="s">
@@ -1377,7 +1378,7 @@
       <c r="J17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="7"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="7:11">
       <c r="G18" s="2" t="s">
@@ -1392,7 +1393,7 @@
       <c r="J18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="7"/>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="7:11">
       <c r="G19" s="2" t="s">
@@ -1407,7 +1408,7 @@
       <c r="J19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="7"/>
+      <c r="K19" s="6"/>
     </row>
     <row r="20" spans="7:11" ht="28.8">
       <c r="G20" s="2" t="s">
@@ -1422,7 +1423,7 @@
       <c r="J20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="7"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="7:11" ht="28.8">
       <c r="G21" s="2" t="s">
@@ -1437,7 +1438,7 @@
       <c r="J21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K21" s="7"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="7:11" ht="28.8">
       <c r="G22" s="2" t="s">
@@ -1452,7 +1453,7 @@
       <c r="J22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="7"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" spans="7:11" ht="43.2">
       <c r="G23" s="2" t="s">
@@ -1467,7 +1468,7 @@
       <c r="J23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="7"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="7:11" ht="27.6">
       <c r="G24" s="2" t="s">
@@ -1482,7 +1483,7 @@
       <c r="J24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="7"/>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="7:11" ht="43.2">
       <c r="G25" s="2" t="s">
@@ -1497,7 +1498,7 @@
       <c r="J25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K25" s="7"/>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" spans="7:11">
       <c r="G26" s="2" t="s">
@@ -1512,7 +1513,7 @@
       <c r="J26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="7"/>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="7:11" ht="43.2">
       <c r="G27" s="2" t="s">
@@ -1527,7 +1528,7 @@
       <c r="J27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K27" s="7"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="7:11" ht="28.8">
       <c r="G28" s="2" t="s">
@@ -1542,7 +1543,7 @@
       <c r="J28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="7"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" spans="7:11" ht="28.8">
       <c r="G29" s="2" t="s">
@@ -1557,7 +1558,7 @@
       <c r="J29" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K29" s="7"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="7:11" ht="28.8">
       <c r="G30" s="2" t="s">
@@ -1572,7 +1573,7 @@
       <c r="J30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K30" s="7"/>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" spans="7:11" ht="28.8">
       <c r="G31" s="2" t="s">
@@ -1587,7 +1588,7 @@
       <c r="J31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K31" s="7"/>
+      <c r="K31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new Features JPG to PDF   ( Working perfectely ) PDF to JPF    ( Working perfectely )
Minor chanegs to the design of the page
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4ACB70-BD26-495F-8150-72C207F9B002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9026B3-A0BC-4FB2-AD10-0060BB0216F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
   <si>
     <t>Feature</t>
   </si>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0084B80B-D593-4AFF-8628-A3ED391DA8B9}">
   <dimension ref="G4:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1348,7 +1348,9 @@
       <c r="J15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="6"/>
+      <c r="K15" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="7:11">
       <c r="G16" s="2" t="s">
@@ -1363,7 +1365,9 @@
       <c r="J16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="6"/>
+      <c r="K16" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="17" spans="7:11" ht="28.8">
       <c r="G17" s="2" t="s">

</xml_diff>

<commit_message>
PDF to Excel Feature added  (  Not working  )
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9026B3-A0BC-4FB2-AD10-0060BB0216F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141EF855-FFA4-4F01-821A-957DC9C15D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
   <si>
     <t>Feature</t>
   </si>
@@ -1141,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0084B80B-D593-4AFF-8628-A3ED391DA8B9}">
   <dimension ref="G4:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1271,7 +1271,9 @@
       <c r="J10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="6"/>
+      <c r="K10" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="7:11" ht="27.6">
       <c r="G11" s="2" t="s">

</xml_diff>

<commit_message>
ADDED FEATURES powerpoint to pdf ( Completed and working )
Excel to Pdf ( 50 % completed need refinement )
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141EF855-FFA4-4F01-821A-957DC9C15D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81554395-E887-4E29-B242-E06ACCC77395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="60">
   <si>
     <t>Feature</t>
   </si>
@@ -746,6 +746,9 @@
   </si>
   <si>
     <t>Processing</t>
+  </si>
+  <si>
+    <t>50% Completed , need refinement</t>
   </si>
 </sst>
 </file>
@@ -1141,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0084B80B-D593-4AFF-8628-A3ED391DA8B9}">
   <dimension ref="G4:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1153,7 +1156,7 @@
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="7:11" ht="28.8">
@@ -1305,9 +1308,11 @@
       <c r="J12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="7:11">
+      <c r="K12" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11" ht="46.8" customHeight="1">
       <c r="G13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1320,7 +1325,9 @@
       <c r="J13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="6"/>
+      <c r="K13" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="7:11" ht="28.8">
       <c r="G14" s="2" t="s">

</xml_diff>

<commit_message>
ADDED features Watermark features added (working) Edit PDF Added ( Only Rectangle Part Working )
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81554395-E887-4E29-B242-E06ACCC77395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C79CE1-0270-487F-A491-41A4A4111FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
   <si>
     <t>Feature</t>
   </si>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0084B80B-D593-4AFF-8628-A3ED391DA8B9}">
   <dimension ref="G4:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1406,7 +1406,9 @@
       <c r="J18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K18" s="6"/>
+      <c r="K18" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="7:11">
       <c r="G19" s="2" t="s">

</xml_diff>

<commit_message>
ADDED NEW Features Rotate PDF ( Working Perfectely )
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C79CE1-0270-487F-A491-41A4A4111FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D79E8C9-20C3-4A58-9421-901B8BB24CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
   <si>
     <t>Feature</t>
   </si>
@@ -1145,7 +1145,7 @@
   <dimension ref="G4:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1423,7 +1423,9 @@
       <c r="J19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="6"/>
+      <c r="K19" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="7:11" ht="28.8">
       <c r="G20" s="2" t="s">

</xml_diff>

<commit_message>
Two  Features added Unlock PDF ( Working 100 % ) Protect PDF ( Not Working )
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D79E8C9-20C3-4A58-9421-901B8BB24CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76FA5C4-50A9-4478-8050-9B52E7E028E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>Feature</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>50% Completed , need refinement</t>
+  </si>
+  <si>
+    <t>Not Working</t>
   </si>
 </sst>
 </file>
@@ -1144,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0084B80B-D593-4AFF-8628-A3ED391DA8B9}">
   <dimension ref="G4:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1455,7 +1458,9 @@
       <c r="J21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K21" s="6"/>
+      <c r="K21" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22" spans="7:11" ht="28.8">
       <c r="G22" s="2" t="s">
@@ -1470,7 +1475,9 @@
       <c r="J22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K22" s="6"/>
+      <c r="K22" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="7:11" ht="43.2">
       <c r="G23" s="2" t="s">

</xml_diff>

<commit_message>
New feature Added Organize PDF - Working 100%
Refined the internal code of Unlock pdf feature .
</commit_message>
<xml_diff>
--- a/requirements_updated.xlsx
+++ b/requirements_updated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\practice full stack web developement\templates\code_pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76FA5C4-50A9-4478-8050-9B52E7E028E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D813737-9F7C-4978-A33E-DB2045931A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035631E5-C6E1-4076-829D-9D00ED10A7DA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="60">
   <si>
     <t>Feature</t>
   </si>
@@ -749,9 +749,6 @@
   </si>
   <si>
     <t>50% Completed , need refinement</t>
-  </si>
-  <si>
-    <t>Not Working</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0084B80B-D593-4AFF-8628-A3ED391DA8B9}">
   <dimension ref="G4:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1476,7 +1473,7 @@
         <v>7</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="7:11" ht="43.2">
@@ -1492,7 +1489,9 @@
       <c r="J23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="24" spans="7:11" ht="27.6">
       <c r="G24" s="2" t="s">

</xml_diff>